<commit_message>
Checks guessing in categorization
</commit_message>
<xml_diff>
--- a/paper/Paper/prev_work.xlsx
+++ b/paper/Paper/prev_work.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\university\mudrick_lab\subliminal_priming_w_motion_capture\paper\Paper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F71CBC68-1C93-42E3-9569-29FD4F9900DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C434223-4F08-455F-A444-F6BA788A6971}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -514,12 +514,6 @@
     <t>Masking
 Prime: picture, Tool / Animal
 Target: picture,Elongatged tool / "blob" like animal
-Task: Categorize as animal / tool</t>
-  </si>
-  <si>
-    <t>Masking
-Prime: picture, Tool / Animal
-Target: picture,Elongatged tool / "blob" like animal
 prime-task: Classify the prime.
                     Separate from main task.
                     Respond with keyboard.</t>
@@ -1149,6 +1143,12 @@
                                   targets.
 Correcting movement length
 correcting movement velocity</t>
+  </si>
+  <si>
+    <t>Masking
+Prime: picture, Tool / Animal of shape Elongated / "blob"
+Target: picture, Elongated tool / "blob" like animal
+Task: Categorize as animal / tool</t>
   </si>
 </sst>
 </file>
@@ -1919,10 +1919,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="F9" sqref="F9"/>
+      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
@@ -1966,10 +1966,10 @@
         <v>77</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>39</v>
@@ -1986,7 +1986,7 @@
         <v>6</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>78</v>
+        <v>126</v>
       </c>
       <c r="E2" t="s">
         <v>7</v>
@@ -1998,11 +1998,11 @@
         <v>10</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I2" s="2"/>
       <c r="J2" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="141.44999999999999" x14ac:dyDescent="0.35">
@@ -2016,25 +2016,25 @@
         <v>6</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E3" t="s">
         <v>9</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="70.75" x14ac:dyDescent="0.35">
@@ -2048,7 +2048,7 @@
         <v>6</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E4" t="s">
         <v>16</v>
@@ -2057,7 +2057,7 @@
         <v>15</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
@@ -2080,19 +2080,19 @@
         <v>7</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="183.9" x14ac:dyDescent="0.35">
@@ -2112,19 +2112,19 @@
         <v>7</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>22</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="238.3" customHeight="1" x14ac:dyDescent="0.35">
@@ -2144,19 +2144,19 @@
         <v>7</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>27</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="210" customHeight="1" x14ac:dyDescent="0.35">
@@ -2170,7 +2170,7 @@
         <v>6</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E8" t="s">
         <v>29</v>
@@ -2179,16 +2179,16 @@
         <v>30</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I8" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="J8" s="5" t="s">
         <v>91</v>
-      </c>
-      <c r="J8" s="5" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="179.15" customHeight="1" x14ac:dyDescent="0.35">
@@ -2205,13 +2205,13 @@
         <v>34</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
@@ -2230,7 +2230,7 @@
         <v>38</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E10" t="s">
         <v>40</v>
@@ -2258,7 +2258,7 @@
         <v>46</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>48</v>
@@ -2314,7 +2314,7 @@
         <v>57</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
@@ -2330,10 +2330,10 @@
         <v>45</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>58</v>
@@ -2342,13 +2342,13 @@
         <v>59</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="240.45" x14ac:dyDescent="0.35">
@@ -2362,10 +2362,10 @@
         <v>60</v>
       </c>
       <c r="D15" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="E15" s="2" t="s">
         <v>96</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>97</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>65</v>
@@ -2374,13 +2374,13 @@
         <v>66</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J15" s="6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="99" x14ac:dyDescent="0.35">
@@ -2394,16 +2394,16 @@
         <v>45</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>69</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
@@ -2419,7 +2419,7 @@
         <v>45</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>51</v>
@@ -2444,7 +2444,7 @@
         <v>45</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>51</v>
@@ -2453,7 +2453,7 @@
         <v>74</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>

</xml_diff>

<commit_message>
Added pre reg progress
</commit_message>
<xml_diff>
--- a/paper/Paper/prev_work.xlsx
+++ b/paper/Paper/prev_work.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\university\mudrick_lab\subliminal_priming_w_motion_capture\paper\Paper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99D5F1DA-9328-429B-938C-A07C3F2A9016}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C94FF4E-1158-448E-9D90-AD672471C4A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="133">
   <si>
     <t>Authors</t>
   </si>
@@ -690,44 +690,6 @@
       <t xml:space="preserve">
 Set size is small (10 targets, 4 primes two of which are also targets)
 Only 80 trials in awareness test
-Awareness test is seperate from main task.
-Didn't use a subjective measure.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Uses keyboard and reaching to show semantic priming
-Exp 1 (b) uses keypress,
-Exp 4 uses reach trajectory,
-Other than that they are the same.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Exp's weakness:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Exp 1 - Half of subjects are aware of the prime,
-             Used only those that were unaware.
-Exp 4 - didn't mention how many were unaware of the prime,
-             Used only those that were unaware.
-In both experiments it can be claimed that the effect is at least partially (if not fully) driven by the shape of the object instead of the category.
-Set size is small (16 primes and 8 targets)
 Awareness test is seperate from main task.
 Didn't use a subjective measure.</t>
     </r>
@@ -1203,6 +1165,49 @@
       </rPr>
       <t>F = 7.4</t>
     </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Uses keyboard and reaching to show semantic priming
+Exp 1 (b) uses keypress,
+Exp 4 uses reach trajectory,
+Other than that they are the same.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Exp's weakness:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Exp 1 - Half of subjects are aware of the prime,
+             Used only those that were unaware. --&gt; regression to the mean = 
+             some "unaware" sybjects are unaware because of measurement 
+              error. They will inflate the unconscious effect.
+Exp 4 - didn't mention how many were unaware of the prime,
+             Used only those that were unaware.
+In both experiments it can be claimed that the effect is at least partially (if not fully) driven by the shape of the object instead of the category.
+Set size is small (16 primes and 8 targets)
+Awareness test is seperate from main task.
+Didn't use a subjective measure.</t>
+    </r>
+  </si>
+  <si>
+    <t>N=58, out of which only 37 were unaware and used for the analysis.</t>
   </si>
 </sst>
 </file>
@@ -1985,10 +1990,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="J8" sqref="J8"/>
+      <selection pane="bottomLeft" activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
@@ -2030,7 +2035,7 @@
         <v>3</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>77</v>
@@ -2045,7 +2050,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="282.89999999999998" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" ht="311.14999999999998" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2056,7 +2061,7 @@
         <v>6</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E2" t="s">
         <v>7</v>
@@ -2071,9 +2076,11 @@
       <c r="I2" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="J2" s="2"/>
+      <c r="J2" s="2" t="s">
+        <v>132</v>
+      </c>
       <c r="K2" s="6" t="s">
-        <v>100</v>
+        <v>131</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="141.44999999999999" x14ac:dyDescent="0.35">
@@ -2087,7 +2094,7 @@
         <v>6</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E3" t="s">
         <v>9</v>
@@ -2096,13 +2103,13 @@
         <v>85</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>81</v>
@@ -2122,7 +2129,7 @@
         <v>6</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E4" t="s">
         <v>16</v>
@@ -2131,7 +2138,7 @@
         <v>15</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
@@ -2158,7 +2165,7 @@
         <v>84</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H5" s="2"/>
       <c r="I5" s="2" t="s">
@@ -2168,7 +2175,7 @@
         <v>82</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="183.9" x14ac:dyDescent="0.35">
@@ -2194,7 +2201,7 @@
         <v>22</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I6" s="2" t="s">
         <v>87</v>
@@ -2203,7 +2210,7 @@
         <v>81</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="238.3" customHeight="1" x14ac:dyDescent="0.35">
@@ -2229,7 +2236,7 @@
         <v>27</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I7" s="2" t="s">
         <v>88</v>
@@ -2238,7 +2245,7 @@
         <v>81</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="210" customHeight="1" x14ac:dyDescent="0.35">
@@ -2252,7 +2259,7 @@
         <v>6</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E8" t="s">
         <v>29</v>
@@ -2261,11 +2268,11 @@
         <v>30</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H8" s="2"/>
       <c r="I8" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="J8" s="2" t="s">
         <v>90</v>
@@ -2291,10 +2298,10 @@
         <v>89</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
@@ -2314,7 +2321,7 @@
         <v>38</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E10" t="s">
         <v>40</v>
@@ -2343,7 +2350,7 @@
         <v>46</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>48</v>
@@ -2401,7 +2408,7 @@
         <v>57</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
@@ -2430,7 +2437,7 @@
         <v>59</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I14" s="4" t="s">
         <v>94</v>
@@ -2439,7 +2446,7 @@
         <v>97</v>
       </c>
       <c r="K14" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="240.45" x14ac:dyDescent="0.35">
@@ -2472,7 +2479,7 @@
         <v>98</v>
       </c>
       <c r="K15" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="99" x14ac:dyDescent="0.35">
@@ -2486,16 +2493,16 @@
         <v>45</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>69</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
@@ -2512,7 +2519,7 @@
         <v>45</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>51</v>
@@ -2538,7 +2545,7 @@
         <v>45</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>51</v>
@@ -2547,7 +2554,7 @@
         <v>74</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>

</xml_diff>